<commit_message>
made enterprise btn base
</commit_message>
<xml_diff>
--- a/Raise the Poor Practice/Assets/xlsx/data.xlsx
+++ b/Raise the Poor Practice/Assets/xlsx/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksh\Documents\raise-the-poor-practice\raise-the-poor-practice\Raise the Poor Practice\Assets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3219E4B-A79E-4577-B7CB-02EAAC819650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8632A2BF-3D73-496E-BDD7-2D34033F4018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="1800" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeit" sheetId="1" r:id="rId1"/>
     <sheet name="Realty" sheetId="2" r:id="rId2"/>
     <sheet name="Paint" sheetId="3" r:id="rId3"/>
+    <sheet name="Enterprise" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,6 +205,66 @@
   </si>
   <si>
     <t>모자라나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테쓸라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bwm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벤츄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폭소바겐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스타박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도요토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>넷플리즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>막도널드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카카콜라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탄센트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이스쿡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아마도존</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이크로하드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애플들</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1148,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD4B5F2-98AA-43CF-BEF1-8728D2F8DCE1}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1321,4 +1382,345 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB846D07-A863-4BB8-BF0C-6BD25AD69B29}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>10000000000000</v>
+      </c>
+      <c r="D2">
+        <v>100000000</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>20000000000000</v>
+      </c>
+      <c r="D3">
+        <v>200000000</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>30000000000000</v>
+      </c>
+      <c r="D4">
+        <v>300000000</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>50000000000000</v>
+      </c>
+      <c r="D5">
+        <v>500000000</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>100000000000000</v>
+      </c>
+      <c r="D6">
+        <v>100000000</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>200000000000000</v>
+      </c>
+      <c r="D7">
+        <v>2000000000</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>300000000000000</v>
+      </c>
+      <c r="D8">
+        <v>3000000000</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>500000000000000</v>
+      </c>
+      <c r="D9">
+        <v>5000000000</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>1000000000000000</v>
+      </c>
+      <c r="D10">
+        <v>10000000000</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>2000000000000000</v>
+      </c>
+      <c r="D11">
+        <v>20000000000</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12">
+        <v>3000000000000000</v>
+      </c>
+      <c r="D12">
+        <v>30000000000</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13">
+        <v>5000000000000000</v>
+      </c>
+      <c r="D13">
+        <v>50000000000</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14">
+        <v>1E+16</v>
+      </c>
+      <c r="D14">
+        <v>100000000000</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15">
+        <v>2E+16</v>
+      </c>
+      <c r="D15">
+        <v>200000000000</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16">
+        <v>3E+16</v>
+      </c>
+      <c r="D16">
+        <v>300000000000</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix arbeit happiness btn
</commit_message>
<xml_diff>
--- a/Raise the Poor Practice/Assets/xlsx/data.xlsx
+++ b/Raise the Poor Practice/Assets/xlsx/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksh\Documents\raise-the-poor-practice\raise-the-poor-practice\Raise the Poor Practice\Assets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C4579E-754F-4D93-9BCE-4609E4A5E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC04115-4F9A-4A3E-87C6-823B6AF73893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeit" sheetId="1" r:id="rId1"/>
@@ -57,22 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>alien_girlfriend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>teacher</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>farmer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>golf_player</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>chief</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -93,46 +77,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fox</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hak</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>frog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bear</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duck</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rabbit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>perSecond</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -330,6 +274,62 @@
   </si>
   <si>
     <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두꺼비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>늑대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>곰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토끼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쥐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돼지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박쥐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -682,13 +682,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>10000</v>
@@ -719,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>50000</v>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>100000</v>
@@ -765,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>500000</v>
@@ -788,7 +788,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>1000000</v>
@@ -811,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>5000000</v>
@@ -834,7 +834,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>10000000</v>
@@ -857,7 +857,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>50000000</v>
@@ -880,7 +880,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>100000000</v>
@@ -903,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>10000000000</v>
@@ -926,7 +926,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="C12">
         <v>50000000000</v>
@@ -949,7 +949,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>100000000000</v>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="C14">
         <v>1000000000000</v>
@@ -995,7 +995,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="C15">
         <v>10000000000000</v>
@@ -1018,7 +1018,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>100000000000000</v>
@@ -1041,7 +1041,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>1000000000000000</v>
@@ -1064,7 +1064,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>5E+18</v>
@@ -1111,16 +1111,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1128,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>200000000</v>
@@ -1148,7 +1148,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>500000000</v>
@@ -1168,7 +1168,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1000000000</v>
@@ -1188,7 +1188,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>2000000000</v>
@@ -1208,7 +1208,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>5000000000</v>
@@ -1228,7 +1228,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>10000000000</v>
@@ -1248,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>100000000000</v>
@@ -1291,16 +1291,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1308,7 +1308,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>200000000000</v>
@@ -1328,7 +1328,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>300000000000</v>
@@ -1348,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>400000000000</v>
@@ -1368,7 +1368,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>500000000000</v>
@@ -1388,7 +1388,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>600000000000</v>
@@ -1408,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>700000000000</v>
@@ -1428,7 +1428,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>40000000000000</v>
@@ -1471,16 +1471,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -1488,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>10000000000000</v>
@@ -1508,7 +1508,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>20000000000000</v>
@@ -1528,7 +1528,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>30000000000000</v>
@@ -1548,7 +1548,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>50000000000000</v>
@@ -1568,7 +1568,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>100000000000000</v>
@@ -1588,7 +1588,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>200000000000000</v>
@@ -1608,7 +1608,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>300000000000000</v>
@@ -1628,7 +1628,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>500000000000000</v>
@@ -1648,7 +1648,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>1000000000000000</v>
@@ -1668,7 +1668,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>2000000000000000</v>
@@ -1688,7 +1688,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>3000000000000000</v>
@@ -1708,7 +1708,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>5000000000000000</v>
@@ -1728,7 +1728,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>1E+16</v>
@@ -1748,7 +1748,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>2E+16</v>
@@ -1768,7 +1768,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>3E+16</v>
@@ -1794,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6B3747-1477-4750-A7C9-BA97A89B5716}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -1811,19 +1811,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -1831,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C2">
         <v>500000000000</v>
@@ -1854,7 +1854,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>600000000000</v>
@@ -1877,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>700000000000</v>
@@ -1900,7 +1900,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>800000000000</v>
@@ -1923,7 +1923,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>900000000000</v>
@@ -1946,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>1000000000000</v>
@@ -1969,7 +1969,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>5000000000000</v>
@@ -1992,7 +1992,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>10000000000000</v>
@@ -2015,7 +2015,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C10">
         <v>50000000000000</v>
@@ -2038,7 +2038,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C11">
         <v>100000000000000</v>
@@ -2061,7 +2061,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C12">
         <v>500000000000000</v>
@@ -2084,7 +2084,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>1000000000000000</v>
@@ -2107,7 +2107,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>5000000000000000</v>
@@ -2130,7 +2130,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C15">
         <v>1E+16</v>
@@ -2153,7 +2153,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>5E+16</v>
@@ -2176,7 +2176,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>1E+17</v>
@@ -2199,7 +2199,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C18">
         <v>5E+17</v>

</xml_diff>

<commit_message>
Poor Power Per Click Update
</commit_message>
<xml_diff>
--- a/Raise the Poor Practice/Assets/xlsx/data.xlsx
+++ b/Raise the Poor Practice/Assets/xlsx/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksh\Documents\raise-the-poor-practice\raise-the-poor-practice\Raise the Poor Practice\Assets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B761A7-780F-45C5-A96B-9A7AA380BF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EA6EB-907B-4EE8-B298-B292A1649DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="1800" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2088" yWindow="1800" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeit" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -728,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1521,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB846D07-A863-4BB8-BF0C-6BD25AD69B29}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1533,7 +1533,7 @@
     <col min="4" max="4" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1552,8 +1552,11 @@
       <c r="F1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1572,8 +1575,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1592,8 +1598,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1612,8 +1621,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1632,8 +1644,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1652,8 +1667,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1672,8 +1690,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G7">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1692,8 +1713,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1712,8 +1736,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1732,8 +1759,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1752,8 +1782,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G11">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1772,8 +1805,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1792,8 +1828,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G13">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1812,8 +1851,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1832,8 +1874,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="G15">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1851,6 +1896,9 @@
       </c>
       <c r="F16">
         <v>0</v>
+      </c>
+      <c r="G16">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add enterprise icon image
</commit_message>
<xml_diff>
--- a/Raise the Poor Practice/Assets/xlsx/data.xlsx
+++ b/Raise the Poor Practice/Assets/xlsx/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksh\Documents\raise-the-poor-practice\raise-the-poor-practice\Raise the Poor Practice\Assets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EA6EB-907B-4EE8-B298-B292A1649DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F3BFA6-F1CD-4A8C-9F42-09DAAA354D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2088" yWindow="1800" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,66 +143,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>테쓸라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bwm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>벤츄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>폭소바겐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스타박스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>도요토</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>넷플리즈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>막도널드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>카카콜라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탄센트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>페이스쿡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아마도존</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이크로하드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>애플들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>lock_status</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -400,6 +340,62 @@
   </si>
   <si>
     <t>양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내팔 프라이팬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맘모스 딱풀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>존슨즈키드 로션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바위 과일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무한크로 락스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백세 배터리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부산 버터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쉬는시간 초코바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>와보래요 오즈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슈퍼 커피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아주라 쿠키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>달표 식용유</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아라리 계란</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닥터미 에너지바</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -766,7 +762,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>10000</v>
@@ -789,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>50000</v>
@@ -812,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>100000</v>
@@ -835,7 +831,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>500000</v>
@@ -858,7 +854,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>1000000</v>
@@ -881,7 +877,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>5000000</v>
@@ -904,7 +900,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <v>10000000</v>
@@ -927,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C9">
         <v>50000000</v>
@@ -950,7 +946,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>100000000</v>
@@ -973,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>10000000000</v>
@@ -996,7 +992,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>50000000000</v>
@@ -1019,7 +1015,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>100000000000</v>
@@ -1042,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>1000000000000</v>
@@ -1065,7 +1061,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C15">
         <v>10000000000000</v>
@@ -1088,7 +1084,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C16">
         <v>100000000000000</v>
@@ -1111,7 +1107,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C17">
         <v>1000000000000000</v>
@@ -1134,7 +1130,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C18">
         <v>5E+18</v>
@@ -1521,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB846D07-A863-4BB8-BF0C-6BD25AD69B29}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1561,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>10000000000000</v>
@@ -1584,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>20000000000000</v>
@@ -1607,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>30000000000000</v>
@@ -1630,7 +1626,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="C5">
         <v>50000000000000</v>
@@ -1653,7 +1649,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="C6">
         <v>100000000000000</v>
@@ -1676,7 +1672,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="C7">
         <v>200000000000000</v>
@@ -1699,7 +1695,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>300000000000000</v>
@@ -1722,7 +1718,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C9">
         <v>500000000000000</v>
@@ -1745,7 +1741,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="C10">
         <v>1000000000000000</v>
@@ -1768,7 +1764,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="C11">
         <v>2000000000000000</v>
@@ -1791,7 +1787,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C12">
         <v>3000000000000000</v>
@@ -1814,7 +1810,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="C13">
         <v>5000000000000000</v>
@@ -1837,7 +1833,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="C14">
         <v>1E+16</v>
@@ -1860,7 +1856,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="C15">
         <v>2E+16</v>
@@ -1876,29 +1872,6 @@
       </c>
       <c r="G15">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16">
-        <v>3E+16</v>
-      </c>
-      <c r="D16">
-        <v>300000000000</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -1941,7 +1914,7 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -1949,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>500000000000</v>
@@ -1972,7 +1945,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>600000000000</v>
@@ -1995,7 +1968,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>700000000000</v>
@@ -2018,7 +1991,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>800000000000</v>
@@ -2041,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>900000000000</v>
@@ -2064,7 +2037,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>1000000000000</v>
@@ -2087,7 +2060,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>5000000000000</v>
@@ -2110,7 +2083,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>10000000000000</v>
@@ -2133,7 +2106,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>50000000000000</v>
@@ -2156,7 +2129,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>100000000000000</v>
@@ -2179,7 +2152,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>500000000000000</v>
@@ -2202,7 +2175,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>1000000000000000</v>
@@ -2225,7 +2198,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>5000000000000000</v>
@@ -2248,7 +2221,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>1E+16</v>
@@ -2271,7 +2244,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>5E+16</v>
@@ -2294,7 +2267,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>1E+17</v>
@@ -2317,7 +2290,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>5E+17</v>
@@ -2380,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1000000000000000</v>
@@ -2400,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>5000000000000000</v>
@@ -2420,7 +2393,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>1E+16</v>
@@ -2440,7 +2413,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <v>5E+16</v>
@@ -2460,7 +2433,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C6">
         <v>1E+17</v>
@@ -2480,7 +2453,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <v>1E+18</v>
@@ -2500,7 +2473,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>1E+19</v>
@@ -2520,7 +2493,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <v>2E+19</v>
@@ -2540,7 +2513,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C10">
         <v>3E+19</v>
@@ -2560,7 +2533,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C11">
         <v>5E+19</v>
@@ -2617,7 +2590,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C2">
         <v>1E+20</v>
@@ -2634,7 +2607,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C3">
         <v>2E+20</v>
@@ -2651,7 +2624,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>3E+20</v>
@@ -2668,7 +2641,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>5E+20</v>
@@ -2685,7 +2658,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>1E+21</v>
@@ -2702,7 +2675,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <v>2E+21</v>
@@ -2719,7 +2692,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C8" s="1">
         <v>3E+21</v>

</xml_diff>